<commit_message>
update excel file and add README.md
</commit_message>
<xml_diff>
--- a/data_perokok_tb.xlsx
+++ b/data_perokok_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\pacmann\sampling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECFACCD-9526-47DC-8135-B485F4481C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28078377-D33C-44B8-B7A7-F4716D308C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{11144E39-2808-42DB-8057-66F86A8BD0BC}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{11144E39-2808-42DB-8057-66F86A8BD0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>KEPULAUAN SERIBU</t>
   </si>
@@ -55,13 +55,19 @@
   </si>
   <si>
     <t>penduduk</t>
+  </si>
+  <si>
+    <t>probability of selection</t>
+  </si>
+  <si>
+    <t>probability of inclusion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +81,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri "/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,10 +124,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,32 +446,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84117203-BEBB-4E3A-8296-BF076F87D740}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="19.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -455,8 +522,41 @@
       <c r="D2" s="2">
         <v>29</v>
       </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2569462</v>
+      </c>
+      <c r="H2" s="1">
+        <v>387218.74249999999</v>
+      </c>
+      <c r="I2" s="2">
+        <v>4462</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.229485238999974</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.64749999999999996</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2569462</v>
+      </c>
+      <c r="O2" s="1">
+        <v>387218.74249999999</v>
+      </c>
+      <c r="P2" s="2">
+        <v>4462</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15.6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -469,8 +569,41 @@
       <c r="D3" s="2">
         <v>4462</v>
       </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1153399</v>
+      </c>
+      <c r="H3" s="1">
+        <v>165788.98510000002</v>
+      </c>
+      <c r="I3" s="2">
+        <v>6670</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.103013021861125</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.35260000000000002</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3234003</v>
+      </c>
+      <c r="O3" s="1">
+        <v>474220.0932</v>
+      </c>
+      <c r="P3" s="2">
+        <v>4126</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="15.6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -483,8 +616,41 @@
       <c r="D4" s="2">
         <v>6670</v>
       </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3234003</v>
+      </c>
+      <c r="H4" s="1">
+        <v>474220.0932</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4126</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.28883709951018299</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.74419999999999997</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1843537</v>
+      </c>
+      <c r="O4" s="1">
+        <v>273636.40590000001</v>
+      </c>
+      <c r="P4" s="2">
+        <v>2662</v>
+      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="15.6">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -497,8 +663,27 @@
       <c r="D5" s="2">
         <v>4207</v>
       </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1843537</v>
+      </c>
+      <c r="H5" s="1">
+        <v>273636.40590000001</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2662</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.16465101606884799</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.5131</v>
+      </c>
+      <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="15.6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -512,7 +697,7 @@
         <v>4126</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="15.6">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -528,5 +713,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>